<commit_message>
workaround for JAR in gitignore
</commit_message>
<xml_diff>
--- a/opentsx-clusters/mmdc-mrc/MDC-MRC.xlsx
+++ b/opentsx-clusters/mmdc-mrc/MDC-MRC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkampf/GITHUB.public/OpenTSx/opentsx-clusters/mmdc-mrc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC67F93E-FB88-3C41-9E51-2992CA5D100C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFBC411-A5A6-7246-A7A3-68368C341ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="1760" windowWidth="28040" windowHeight="13740" xr2:uid="{183DE6D2-7FE4-EA4F-8A21-BAAE338FD231}"/>
+    <workbookView xWindow="3320" yWindow="1760" windowWidth="28040" windowHeight="13740" activeTab="2" xr2:uid="{183DE6D2-7FE4-EA4F-8A21-BAAE338FD231}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="3" r:id="rId1"/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07AFDD6-7DEF-E24E-B47E-A54253F2B46D}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B1B1B0-6AC5-F142-BF7D-D83768C7017F}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>